<commit_message>
optimizacion de las fechas
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,7 +583,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2024-05-05</t>
         </is>
       </c>
     </row>
@@ -668,6 +668,34 @@
       <c r="F9" t="inlineStr">
         <is>
           <t>2024-01-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ivan</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>gorda</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>460036</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>8675309125</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2024-12-11</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
editar y borrar funcionando
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,7 +583,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-05-05</t>
+          <t>2026-03-05</t>
         </is>
       </c>
     </row>
@@ -617,20 +617,20 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>gua</t>
+          <t>ivan</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>fer</t>
+          <t>gorda</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>124578</v>
+        <v>460036</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -638,62 +638,6 @@
         </is>
       </c>
       <c r="F8" t="inlineStr">
-        <is>
-          <t>2024-01-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>maxi</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>morales</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>9999</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>8675309125</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2024-01-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>ivan</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>gorda</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>460036</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>8675309125</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
         <is>
           <t>2024-12-11</t>
         </is>

</xml_diff>

<commit_message>
lectura digital funcionando correctamente, falta parte de arduino y el envio desde la pc a arduino, hasrwarey a vender loco
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,20 +533,20 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>lucia</t>
+          <t>francisco</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ferrero</t>
+          <t>mezardo</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>47470000</v>
+        <v>46329841</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -555,26 +555,26 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-02-05</t>
+          <t>2026-03-05</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>francisco</t>
+          <t>javier</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>mezas</t>
+          <t>milei</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>46329841</v>
+        <v>99999999</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -583,26 +583,26 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2026-03-05</t>
+          <t>2023-12-06</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>javier</t>
+          <t>ivan</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>milei</t>
+          <t>gorda</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>99999999</v>
+        <v>460036</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -611,35 +611,91 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-12-06</t>
+          <t>2024-12-11</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ivan</t>
+          <t>fran</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>gorda</t>
+          <t>gg</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>460036</v>
+        <v>8574</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>8675309125</t>
+          <t>46329841</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2024-12-11</t>
+          <t>2023-12-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TIZI</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>dio</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1256</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>12313</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2024-12-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>13</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>luc</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ferrero</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>47470000</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>16050520</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2024-12-20</t>
         </is>
       </c>
     </row>

</xml_diff>